<commit_message>
stand 04 11 2025
</commit_message>
<xml_diff>
--- a/MiniArcade_Documentation/Pin_Out_MiniArcade.xlsx
+++ b/MiniArcade_Documentation/Pin_Out_MiniArcade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MiniArcade\MiniArcadePCB\MiniArcade_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858C34F2-C1B6-4AF7-92EB-63C532F4B805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7803D2B7-38A7-4807-B753-3AC97D27E893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{25E6525B-88BE-4E83-B9F8-2D92674FB24F}"/>
   </bookViews>
@@ -92,15 +92,6 @@
     <t>PB05</t>
   </si>
   <si>
-    <t>PB03</t>
-  </si>
-  <si>
-    <t>PB02</t>
-  </si>
-  <si>
-    <t>PB01</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -113,15 +104,6 @@
     <t>Low</t>
   </si>
   <si>
-    <t>PB00</t>
-  </si>
-  <si>
-    <t>PB06</t>
-  </si>
-  <si>
-    <t>PB07</t>
-  </si>
-  <si>
     <t>Device:</t>
   </si>
   <si>
@@ -138,6 +120,24 @@
   </si>
   <si>
     <t>LCD_RESET</t>
+  </si>
+  <si>
+    <t>PA00</t>
+  </si>
+  <si>
+    <t>PA01</t>
+  </si>
+  <si>
+    <t>PA02</t>
+  </si>
+  <si>
+    <t>PB09</t>
+  </si>
+  <si>
+    <t>PB08</t>
+  </si>
+  <si>
+    <t>PA03</t>
   </si>
 </sst>
 </file>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6835475A-D682-41CE-B56A-665B51D5A123}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,13 +550,13 @@
         <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -610,7 +610,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H4">
         <v>80</v>
@@ -629,7 +629,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -665,10 +665,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -682,10 +682,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -714,10 +714,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -822,7 +822,7 @@
         <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E18" s="1"/>
     </row>
@@ -834,13 +834,13 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -867,10 +867,10 @@
         <v>11</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -884,7 +884,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -899,10 +899,10 @@
         <v>12</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -959,7 +959,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E27" s="1"/>
     </row>

</xml_diff>